<commit_message>
x1049 addition: support xenium barcode (prebarcode) in file slide reg
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/section_reg.xlsx
+++ b/src/test/resources/testdata/section_reg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dr6/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dr6/Code/stan/core/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F0803A2-48F1-5C49-8F9E-02D4ED2E839F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87F08FC-D66D-1E4C-8968-F685371B2185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2800" windowWidth="27640" windowHeight="16940" activeTab="3"/>
+    <workbookView xWindow="16160" yWindow="3520" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <r>
       <t xml:space="preserve">SGP number
@@ -386,26 +386,25 @@
   </si>
   <si>
     <t>X903</t>
+  </si>
+  <si>
+    <t>Xenium slide barcode (…)</t>
+  </si>
+  <si>
+    <t>ABC1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -594,55 +593,55 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -958,7 +957,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -970,7 +969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -982,7 +981,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -994,17 +993,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" ht="115" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:19" ht="115" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,49 +1014,52 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
@@ -1067,46 +1069,47 @@
       <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>23</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>1</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12">
         <v>4</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="10">
+      <c r="R3" s="12"/>
+      <c r="S3" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>28</v>
       </c>
@@ -1117,49 +1120,52 @@
         <v>30</v>
       </c>
       <c r="E4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="M4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="17">
+      <c r="N4" s="17">
         <v>3</v>
       </c>
-      <c r="N4" s="17">
+      <c r="O4" s="17">
         <v>4</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="17">
+      <c r="Q4" s="17">
         <v>12</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="R4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="13">
+      <c r="S4" s="13">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>38</v>
       </c>
@@ -1169,44 +1175,45 @@
       <c r="D5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="J5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="K5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="M5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="17">
+      <c r="N5" s="17">
         <v>0</v>
       </c>
-      <c r="N5" s="17">
+      <c r="O5" s="17">
         <v>1</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="P5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="P5" s="17">
+      <c r="Q5" s="17">
         <v>124</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="13"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>